<commit_message>
Tue Feb 18 06:50:04 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary/workflow_types.xlsx
+++ b/bosai/summary/workflow_types.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+  <si>
+    <t xml:space="preserve">Class</t>
+  </si>
   <si>
     <t xml:space="preserve">Status</t>
   </si>
@@ -23,367 +26,382 @@
     <t xml:space="preserve">id_title</t>
   </si>
   <si>
+    <t xml:space="preserve">基因集数据库调用</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finished</t>
   </si>
   <si>
-    <t xml:space="preserve">m6A 编辑位点获取</t>
+    <t xml:space="preserve">m6A 编辑位点获取[gene]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL240914 (预测甲基化调控因子)</t>
   </si>
   <si>
-    <t xml:space="preserve">从 GEO 挖掘可用数据:RNA-seq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSCL241113 (再生障碍性贫血), BSCL241113 (再生障碍性贫血), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (线粒体自噬), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性), BSXN240936 (高级别浆液性卵巢癌)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limma, edgeR 差异分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSCL241113 (再生障碍性贫血), BSHQ230805 (膀胱癌), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSHQ240813 (黑色素瘤), BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (线粒体自噬), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性), BSXN240936 (高级别浆液性卵巢癌)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEGG、GO富集分析</t>
+    <t xml:space="preserve">RNA-seq 或 Microarray 等数据分析涉及的方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从 GEO 挖掘可用数据:RNA-seq[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSCL241113 (再生障碍性贫血), BSCL241113 (再生障碍性贫血), BSGY240816 (结肠癌), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (线粒体自噬), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性), BSXN240936 (高级别浆液性卵巢癌)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limma, edgeR 差异分析[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSCL241113 (再生障碍性贫血), BSGY240816 (结肠癌), BSHQ230805 (膀胱癌), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSHQ240813 (黑色素瘤), BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (线粒体自噬), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性), BSXN240936 (高级别浆液性卵巢癌)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEGG、GO富集分析[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSCL241113 (再生障碍性贫血), BSHQ230805 (膀胱癌), BSHQ240813 (黑色素瘤), BSJF240734 (清心莲子饮网络药理学分析), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXG250204 (多酚五种成分与高脂血症网络药理分析)</t>
   </si>
   <si>
-    <t xml:space="preserve">表观遗传调控因子数据获取 (数据库)</t>
+    <t xml:space="preserve">表观遗传调控因子数据获取 (数据库)[gene]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSJF250113 (消瘀泄浊饮对糖尿病肾病), BSXN240936 (高级别浆液性卵巢癌)</t>
   </si>
   <si>
-    <t xml:space="preserve">蛋白转录后修饰位点预测 (PTMs)</t>
+    <t xml:space="preserve">蛋白转录后修饰位点预测 (PTMs)[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL240914 (预测甲基化调控因子), BSXL240708 (卵巢癌耐药性)</t>
   </si>
   <si>
-    <t xml:space="preserve">TWAS全转录组关联研究</t>
+    <t xml:space="preserve">TWAS全转录组关联研究[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL241113 (再生障碍性贫血)</t>
   </si>
   <si>
-    <t xml:space="preserve">单细胞拟时分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">单细胞数据分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">变异注释 (SNP 获取 rsID 等注释)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GWAS 数据获取和分析</t>
+    <t xml:space="preserve">单细胞数据分析[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WES 或 WGS 或 GWAS 其他涉及基因变异的分析方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">变异注释 (SNP 获取 rsID 等注释)[snp-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scRNA-seq 或 ST 分析涉及的方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">单细胞拟时分析[scrna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWAS 数据获取和分析[snp-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL241113 (再生障碍性贫血), BSCL241113 (再生障碍性贫血)</t>
   </si>
   <si>
-    <t xml:space="preserve">GEO 数据库搜索、调研，获取可用数据</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSCL241113 (再生障碍性贫血), BSJF250113 (线粒体自噬), BSLL241244 (睡眠呼吸暂停症+间歇性低氧诱导的动物模型), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性), BSXN240936 (高级别浆液性卵巢癌), BSYB250111 (骨质疏松)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">单细胞数据预测代谢通量</t>
+    <t xml:space="preserve">其他方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEO 数据库搜索、调研，获取可用数据[other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSCL241113 (再生障碍性贫血), BSGY240816 (结肠癌), BSJF250113 (线粒体自噬), BSLL241244 (睡眠呼吸暂停症+间歇性低氧诱导的动物模型), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性), BSXN240936 (高级别浆液性卵巢癌), BSYB250111 (骨质疏松)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">单细胞数据预测代谢通量[scrna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSCL241113 (再生障碍性贫血), BSZD231122 (骨肉瘤)</t>
   </si>
   <si>
-    <t xml:space="preserve">TCGA 数据挖掘和常规分析 (下载和整理)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSHQ230805 (膀胱癌), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSHQ240813 (黑色素瘤), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">生存分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomaRt 基因注释、信息获取</t>
+    <t xml:space="preserve">TCGA 数据挖掘和常规分析 (下载和整理)[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSGY240816 (结肠癌), BSHQ230805 (膀胱癌), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSHQ240813 (黑色素瘤), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXL240708 (卵巢癌耐药性)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生存分析[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCSCXenaTools 癌症相关数据获取 (相较于 TCGA 补充了 GTEx 和 Target 数据库，适合 Cancer VS Normal)[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSGY240816 (结肠癌), BSHQ240813 (黑色素瘤)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomaRt 基因注释、信息获取[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSHQ230805 (膀胱癌), BSHQ240303 (骨肉瘤分析ZDHHC家族成员), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物), BSXN240936 (高级别浆液性卵巢癌)</t>
   </si>
   <si>
-    <t xml:space="preserve">GSEA 富集分析</t>
+    <t xml:space="preserve">GSEA 富集分析[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSHQ230805 (膀胱癌), BSHQ240813 (黑色素瘤)</t>
   </si>
   <si>
-    <t xml:space="preserve">构建 PPI 网络</t>
+    <t xml:space="preserve">构建 PPI 网络[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSHQ230805 (膀胱癌), BSHQ240813 (黑色素瘤), BSXG250204 (多酚五种成分与高脂血症网络药理分析), BSXL240708 (卵巢癌耐药性)</t>
   </si>
   <si>
-    <t xml:space="preserve">UCSCXenaTools 癌症相关数据获取 (相较于 TCGA 补充了 GTEx 和 Target 数据库，适合 Cancer VS Normal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSHQ240813 (黑色素瘤)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEGG 通路可视化和表达量映射</t>
+    <t xml:space="preserve">KEGG 通路可视化和表达量映射[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSHQ240813 (黑色素瘤), BSJF240734 (清心莲子饮网络药理学分析), BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物)</t>
   </si>
   <si>
-    <t xml:space="preserve">铁死亡相关基因挖掘</t>
+    <t xml:space="preserve">铁死亡相关基因挖掘[gene]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF240734 (清心莲子饮网络药理学分析)</t>
   </si>
   <si>
-    <t xml:space="preserve">获取疾病或条件相关的基因集:Genecards</t>
+    <t xml:space="preserve">获取疾病或条件相关的基因集:Genecards[gene]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (消瘀泄浊饮对糖尿病肾病), BSJF250113 (线粒体自噬), BSXG250204 (多酚五种成分与高脂血症网络药理分析)</t>
   </si>
   <si>
-    <t xml:space="preserve">挖掘 BATMAN (网络药理学) 数据库</t>
+    <t xml:space="preserve">网络药理学方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">挖掘 BATMAN (网络药理学) 数据库[pharm]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (消瘀泄浊饮对糖尿病肾病), BSXG250204 (多酚五种成分与高脂血症网络药理分析)</t>
   </si>
   <si>
-    <t xml:space="preserve">20% HOB 口服生物利用度预测</t>
-  </si>
-  <si>
-    <t xml:space="preserve">全自动批量分子对接</t>
+    <t xml:space="preserve">20% HOB 口服生物利用度预测[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">全自动批量分子对接[pharm]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF240734 (清心莲子饮网络药理学分析), BSJF250113 (消瘀泄浊饮对糖尿病肾病), BSXL240708 (卵巢癌耐药性)</t>
   </si>
   <si>
-    <t xml:space="preserve">RBP 预测:RNA 结合蛋白与 RNA 的结合</t>
+    <t xml:space="preserve">RBP 预测:RNA 结合蛋白与 RNA 的结合[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF250113 (消瘀泄浊饮对糖尿病肾病)</t>
   </si>
   <si>
-    <t xml:space="preserve">取交集</t>
+    <t xml:space="preserve">取交集[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF250113 (消瘀泄浊饮对糖尿病肾病), BSJF250113 (线粒体自噬), BSXN240936 (高级别浆液性卵巢癌)</t>
   </si>
   <si>
-    <t xml:space="preserve">LncRNA调控靶点</t>
+    <t xml:space="preserve">LncRNA调控靶点[gene]</t>
   </si>
   <si>
     <t xml:space="preserve">BSJF250113 (线粒体自噬)</t>
   </si>
   <si>
-    <t xml:space="preserve">构建 LASSO-COX 预后模型</t>
+    <t xml:space="preserve">构建 LASSO-COX 预后模型[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSXG240327 (基于血小板RNA测序数据预测早期肺癌潜在生物标志物)</t>
   </si>
   <si>
-    <t xml:space="preserve">对基因聚类分析 (时序分析) mfuzz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WGCNA 共表达分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClusPro 蛋白质与蛋白质之间的对接模拟</t>
+    <t xml:space="preserve">对基因聚类分析 (时序分析) mfuzz[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGCNA 共表达分析[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClusPro 蛋白质与蛋白质之间的对接模拟[rna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSXL240708 (卵巢癌耐药性)</t>
   </si>
   <si>
-    <t xml:space="preserve">单细胞数据分析注释细胞群</t>
+    <t xml:space="preserve">单细胞数据分析注释细胞群[scrna-method]</t>
   </si>
   <si>
     <t xml:space="preserve">BSZD231122 (骨肉瘤)</t>
   </si>
   <si>
-    <t xml:space="preserve">单细胞数据鉴定癌细胞 (copyKAT)</t>
+    <t xml:space="preserve">单细胞数据鉴定癌细胞 (copyKAT)[scrna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16s RNA-seq 肠道菌群测序数据分析</t>
   </si>
   <si>
     <t xml:space="preserve">Not Finished</t>
   </si>
   <si>
-    <t xml:space="preserve">常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">circRNA 结合 miRNA 位点预测</t>
-  </si>
-  <si>
-    <t xml:space="preserve">miRNA 结合 mRNA 位点预测</t>
-  </si>
-  <si>
-    <t xml:space="preserve">基因组比对:Bowtie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">空间代谢组数据分析:Cardinal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">化合物系统分类注释 (ClassyFire) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">化合物信息获取:同义名、smiles、inchikey等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CpG islands 数据获取</t>
-  </si>
-  <si>
-    <t xml:space="preserve">编写爬虫工具批量获取网页数据</t>
-  </si>
-  <si>
-    <t xml:space="preserve">化合物和疾病关联数据获取 (CTD 数据库)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HERB (网络药理学) 数据库</t>
-  </si>
-  <si>
-    <t xml:space="preserve">从 Plantaedb 数据库获取植物成分信息 (作为中药数据库缺失记录的补充) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCMSP (网络药理学) 数据库数据挖掘</t>
-  </si>
-  <si>
-    <t xml:space="preserve">分子对接肽与蛋白</t>
-  </si>
-  <si>
-    <t xml:space="preserve">全自动批量分子对接 (从蛋白质、分子名字到对接结果)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">代谢物富集分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathview 可视化富集通路</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fastq 文件预处理、对齐参考基因</t>
-  </si>
-  <si>
-    <t xml:space="preserve">铁死亡相关基因获取 (数据库)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">从头开始的 LC-MS/MS 数据处理:数据格式转换、峰检测、化合物鉴定等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LC-MS/MS 数据深入分析:差异代谢物筛选、分子网络可视化、富集分析等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LC-MS/MS 数据以尖端预测工具鉴定更多化合物 (费时)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">基因 (RNA) 和 eQTL 关联性挖掘:通过公共数据 (文献的补充材料)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">蛋白质或基因和代谢物数据联合分析:通过公共数据挖掘建立联系 (文献的补充材料)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">蛋白质或基因、肠道菌群、代谢物数据联合分析:通过公共数据 (文献的补充材料)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系 (文献的补充材料)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">结合不同 (如疾病) 条件下 RNA-seq DEGs 筛选基因</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bibliometrix 常规文献计量分析和可视化</t>
-  </si>
-  <si>
-    <t xml:space="preserve">变异注释分析和可视化:maftools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">质谱数据分析:原始数据预处理、特征峰解卷积等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">代谢物数据分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">宏基因组数据分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">甲基化芯片数据分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">差异甲基化分析、可视化</t>
-  </si>
-  <si>
-    <t xml:space="preserve">批量 OCR 识别图片中文字并整理结果</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRINGdb 构建 PPI 网络</t>
-  </si>
-  <si>
-    <t xml:space="preserve">药物临床化疗反应预测、耐药性预测</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PubMed 文献搜索</t>
-  </si>
-  <si>
-    <t xml:space="preserve">蛋白质 pdb 数据 (PDB，AlphaFold 互为补充) 获取用于可视化</t>
-  </si>
-  <si>
-    <t xml:space="preserve">蛋白质信息获取</t>
-  </si>
-  <si>
-    <t xml:space="preserve">从头开始的 RNA-seq 数据分析:从原始数据 fastq 开始质控、注释等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCGA RNA-seq 数据挖掘和常规分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">从头开始的 RNA-seq 数据分析:从 fastq 开始质控、注释等</t>
-  </si>
-  <si>
-    <t xml:space="preserve">制作特定功能的 R 包</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCSA、ChatGPT-4 细胞注释</t>
-  </si>
-  <si>
-    <t xml:space="preserve">单细胞数据细胞注释到具体细胞亚群:如 Treg 细胞</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CellChat 单细胞细胞通讯</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monocle3 拟时分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">空间转录组常规分析 (大致同单细胞数据) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">以拟时分析区分细胞亚群</t>
-  </si>
-  <si>
-    <t xml:space="preserve">数据库获取化合物靶点</t>
-  </si>
-  <si>
-    <t xml:space="preserve">预测化合物靶点</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SwissTargetPrediction 预测化合物靶点 (限制访问)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCGA 变异数据 (Variant) 挖掘和常规分析</t>
-  </si>
-  <si>
-    <t xml:space="preserve">调控该基因的相关转录因子 (TF) 数据获取</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UCSC table 数据获取、基因位点注释</t>
-  </si>
-  <si>
-    <t xml:space="preserve">跨膜蛋白数据获取</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WES 变异筛选</t>
-  </si>
-  <si>
-    <t xml:space="preserve">从头开始的 WES 数据分析:从 fastq 开始质控、注释等</t>
+    <t xml:space="preserve">常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等[16s-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">circRNA 结合 miRNA 位点预测[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miRNA 结合 mRNA 位点预测[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathview 可视化富集通路[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRINGdb 构建 PPI 网络[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蛋白质信息获取[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGA RNA-seq 数据挖掘和常规分析[rna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">变异注释分析和可视化:maftools[snp-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGA 变异数据 (Variant) 挖掘和常规分析[snp-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WES 变异筛选[snp-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCSA、ChatGPT-4 细胞注释[scrna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellChat 单细胞细胞通讯[scrna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monocle3 拟时分析[scrna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">空间转录组常规分析 (大致同单细胞数据) [scrna-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从原始数据开始的 RNA-seq 数据分析</t>
+  </si>
+  <si>
+    <t xml:space="preserve">基因组比对:Bowtie 2[raw-rna]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastq 文件预处理、对齐参考基因[raw-rna]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宏基因组数据分析[raw-rna]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从头开始的 RNA-seq 数据分析:从原始数据 fastq 开始质控、注释等[raw-rna]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从头开始的 RNA-seq 数据分析:从 fastq 开始质控、注释等[raw-rna]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从原始数据开始的 WES 或 WGS 数据分析</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从头开始的 WES 数据分析:从 fastq 开始质控、注释等[raw-snp]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从原始数据开始的代谢组数据分析</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从头开始的 LC-MS/MS 数据处理:数据格式转换、峰检测、化合物鉴定等[raw-mb]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代谢组或代谢物数据分析方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">空间代谢组数据分析:Cardinal[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">化合物系统分类注释 (ClassyFire) [mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">化合物信息获取:同义名、smiles、inchikey等[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代谢物富集分析[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC-MS/MS 数据深入分析:差异代谢物筛选、分子网络可视化、富集分析等[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC-MS/MS 数据以尖端预测工具鉴定更多化合物 (费时)[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">质谱数据分析:原始数据预处理、特征峰解卷积等[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代谢物数据分析[mb-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">编写爬虫工具批量获取网页数据[other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibliometrix 常规文献计量分析和可视化[other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">批量 OCR 识别图片中文字并整理结果[other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PubMed 文献搜索[other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">制作特定功能的 R 包[other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">化合物和疾病关联数据获取 (CTD 数据库)[gene]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">铁死亡相关基因获取 (数据库)[gene]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">调控该基因的相关转录因子 (TF) 数据获取[gene]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">跨膜蛋白数据获取[gene]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">甲基化测序数据分析方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CpG islands 数据获取[me-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">甲基化芯片数据分析[me-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">差异甲基化分析、可视化[me-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCSC table 数据获取、基因位点注释[me-method]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HERB (网络药理学) 数据库[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从 Plantaedb 数据库获取植物成分信息 (作为中药数据库缺失记录的补充)[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCMSP (网络药理学) 数据库数据挖掘[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">分子对接肽与蛋白[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">全自动批量分子对接 (从蛋白质、分子名字到对接结果)[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">药物临床化疗反应预测、耐药性预测[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蛋白质 pdb 数据 (PDB，AlphaFold 互为补充) 获取用于可视化[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">数据库获取化合物靶点[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">预测化合物靶点[pharm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SwissTargetPrediction 预测化合物靶点 (限制访问)[pharm]</t>
   </si>
 </sst>
 </file>
@@ -725,929 +743,1133 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36"/>
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37"/>
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38"/>
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39"/>
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40"/>
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41"/>
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42"/>
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
         <v>72</v>
       </c>
-      <c r="C43"/>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44"/>
+        <v>72</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45"/>
+        <v>72</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46"/>
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47"/>
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48"/>
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49"/>
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49"/>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50"/>
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51"/>
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52"/>
+        <v>72</v>
+      </c>
+      <c r="C52" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53"/>
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54"/>
+        <v>72</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55"/>
+        <v>72</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56"/>
+        <v>72</v>
+      </c>
+      <c r="C56" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57"/>
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57"/>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58"/>
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58"/>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59"/>
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60"/>
+        <v>72</v>
+      </c>
+      <c r="C60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61"/>
+        <v>72</v>
+      </c>
+      <c r="C61" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62"/>
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
-      </c>
-      <c r="C63"/>
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64"/>
+        <v>72</v>
+      </c>
+      <c r="C64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65"/>
+        <v>72</v>
+      </c>
+      <c r="C65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65"/>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66"/>
+        <v>72</v>
+      </c>
+      <c r="C66" t="s">
+        <v>101</v>
+      </c>
+      <c r="D66"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
-      </c>
-      <c r="C67"/>
+        <v>72</v>
+      </c>
+      <c r="C67" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68"/>
+        <v>72</v>
+      </c>
+      <c r="C68" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69"/>
+        <v>72</v>
+      </c>
+      <c r="C69" t="s">
+        <v>108</v>
+      </c>
+      <c r="D69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70"/>
+        <v>72</v>
+      </c>
+      <c r="C70" t="s">
+        <v>109</v>
+      </c>
+      <c r="D70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
-      </c>
-      <c r="C71"/>
+        <v>72</v>
+      </c>
+      <c r="C71" t="s">
+        <v>110</v>
+      </c>
+      <c r="D71"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
-      </c>
-      <c r="C72"/>
+        <v>72</v>
+      </c>
+      <c r="C72" t="s">
+        <v>111</v>
+      </c>
+      <c r="D72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>101</v>
-      </c>
-      <c r="C73"/>
+        <v>72</v>
+      </c>
+      <c r="C73" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
-      </c>
-      <c r="C74"/>
+        <v>72</v>
+      </c>
+      <c r="C74" t="s">
+        <v>113</v>
+      </c>
+      <c r="D74"/>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>103</v>
-      </c>
-      <c r="C75"/>
+        <v>72</v>
+      </c>
+      <c r="C75" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>104</v>
-      </c>
-      <c r="C76"/>
+        <v>72</v>
+      </c>
+      <c r="C76" t="s">
+        <v>116</v>
+      </c>
+      <c r="D76"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>105</v>
-      </c>
-      <c r="C77"/>
+        <v>72</v>
+      </c>
+      <c r="C77" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77"/>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
-      </c>
-      <c r="C78"/>
+        <v>72</v>
+      </c>
+      <c r="C78" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78"/>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
-      </c>
-      <c r="C79"/>
+        <v>72</v>
+      </c>
+      <c r="C79" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
-      </c>
-      <c r="C80"/>
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80"/>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B81" t="s">
-        <v>109</v>
-      </c>
-      <c r="C81"/>
+        <v>72</v>
+      </c>
+      <c r="C81" t="s">
+        <v>121</v>
+      </c>
+      <c r="D81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B82" t="s">
-        <v>110</v>
-      </c>
-      <c r="C82"/>
+        <v>72</v>
+      </c>
+      <c r="C82" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82"/>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
-      </c>
-      <c r="C83"/>
+        <v>72</v>
+      </c>
+      <c r="C83" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83"/>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
-      </c>
-      <c r="C84"/>
+        <v>72</v>
+      </c>
+      <c r="C84" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C85"/>
+        <v>72</v>
+      </c>
+      <c r="C85" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B86" t="s">
-        <v>113</v>
-      </c>
-      <c r="C86"/>
+        <v>72</v>
+      </c>
+      <c r="C86" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
-      </c>
-      <c r="C87"/>
+        <v>72</v>
+      </c>
+      <c r="C87" t="s">
+        <v>127</v>
+      </c>
+      <c r="D87"/>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B88" t="s">
-        <v>115</v>
-      </c>
-      <c r="C88"/>
+        <v>72</v>
+      </c>
+      <c r="C88" t="s">
+        <v>128</v>
+      </c>
+      <c r="D88"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B89" t="s">
-        <v>116</v>
-      </c>
-      <c r="C89"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>64</v>
-      </c>
-      <c r="B90" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>64</v>
-      </c>
-      <c r="B91" t="s">
-        <v>118</v>
-      </c>
-      <c r="C91"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>64</v>
-      </c>
-      <c r="B92" t="s">
-        <v>119</v>
-      </c>
-      <c r="C92"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>64</v>
-      </c>
-      <c r="B93" t="s">
-        <v>120</v>
-      </c>
-      <c r="C93"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>64</v>
-      </c>
-      <c r="B94" t="s">
-        <v>121</v>
-      </c>
-      <c r="C94"/>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>64</v>
-      </c>
-      <c r="B95" t="s">
-        <v>122</v>
-      </c>
-      <c r="C95"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>64</v>
-      </c>
-      <c r="B96" t="s">
-        <v>123</v>
-      </c>
-      <c r="C96"/>
+        <v>72</v>
+      </c>
+      <c r="C89" t="s">
+        <v>129</v>
+      </c>
+      <c r="D89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>